<commit_message>
Second commit with all testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="UserManagementModule" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -107,9 +107,6 @@
     <t>AlphabeticInputName</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>NumericInputName</t>
   </si>
   <si>
@@ -134,10 +131,28 @@
     <t>InvalidUserName</t>
   </si>
   <si>
-    <t>Sunidhi</t>
-  </si>
-  <si>
-    <t>sunidhi@gmail.com</t>
+    <t>Simran</t>
+  </si>
+  <si>
+    <t>Indore I</t>
+  </si>
+  <si>
+    <t>UserManagementPageRole</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>UsernameInUNPage</t>
+  </si>
+  <si>
+    <t>IBU0001192</t>
+  </si>
+  <si>
+    <t>Mahalinga</t>
+  </si>
+  <si>
+    <t>mahalinga@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -553,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,9 +594,12 @@
     <col min="18" max="18" width="24" customWidth="1"/>
     <col min="19" max="20" width="11.85546875" customWidth="1"/>
     <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="11.85546875" customWidth="1"/>
+    <col min="23" max="23" width="26.28515625" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -631,22 +649,31 @@
         <v>26</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -654,10 +681,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2">
         <v>8089889910</v>
@@ -693,22 +720,31 @@
         <v>90089257</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="2">
         <v>12345</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="U2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Collection Agency Role Management testcase scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserManagementModule" sheetId="3" r:id="rId1"/>
+    <sheet name="CollectionAgency" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -153,13 +154,47 @@
   </si>
   <si>
     <t>mahalinga@gmail.com</t>
+  </si>
+  <si>
+    <t>Role Name</t>
+  </si>
+  <si>
+    <t>TC_ProcessSheet_CollectionAgency</t>
+  </si>
+  <si>
+    <t>Role5</t>
+  </si>
+  <si>
+    <t>AlphanumericName</t>
+  </si>
+  <si>
+    <t>Role25</t>
+  </si>
+  <si>
+    <t>specialCharacters</t>
+  </si>
+  <si>
+    <r>
+      <t>^</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>%$</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +214,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -570,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -755,4 +798,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
User management module testscripts
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="6135"/>
   </bookViews>
   <sheets>
     <sheet name="UserManagementModule" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -188,6 +188,18 @@
       </rPr>
       <t>%$</t>
     </r>
+  </si>
+  <si>
+    <t>PwdOriginal</t>
+  </si>
+  <si>
+    <t>UNOriginal</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>IBU0001195</t>
   </si>
 </sst>
 </file>
@@ -269,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -295,6 +307,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -611,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,9 +655,11 @@
     <col min="22" max="22" width="11.85546875" customWidth="1"/>
     <col min="23" max="23" width="26.28515625" customWidth="1"/>
     <col min="24" max="24" width="18.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -715,8 +732,14 @@
       <c r="X1" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -788,15 +811,22 @@
       </c>
       <c r="X2" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="Z2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -804,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>